<commit_message>
CLI: update CSV/Excel input templates
</commit_message>
<xml_diff>
--- a/illumio_pylo/utilities/resources/workloads-import-example.xlsx
+++ b/illumio_pylo/utilities/resources/workloads-import-example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://illumio-my.sharepoint.com/personal/christophe_painchaud_illumio_com/Documents/Synced/dev/pylo/utilities/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christophe.painchaud\Documents\repos\pylo-workdir\pylo\illumio_pylo\utilities\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{63639AB7-BB7A-44F0-8117-10C69E46CEA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A5A6E8C0-93DD-42CE-B992-703D38B475BC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9963C6BA-3693-480E-B0D2-46896EE95DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="workloads-import-example" sheetId="1" r:id="rId1"/>
@@ -31,18 +31,6 @@
     <t>ip</t>
   </si>
   <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>app</t>
-  </si>
-  <si>
-    <t>env</t>
-  </si>
-  <si>
-    <t>loc</t>
-  </si>
-  <si>
     <t>VEN-KFMG</t>
   </si>
   <si>
@@ -62,6 +50,18 @@
   </si>
   <si>
     <t>L_AMER</t>
+  </si>
+  <si>
+    <t>label:role</t>
+  </si>
+  <si>
+    <t>label:app</t>
+  </si>
+  <si>
+    <t>label:env</t>
+  </si>
+  <si>
+    <t>label:loc</t>
   </si>
 </sst>
 </file>
@@ -606,9 +606,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -646,7 +646,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -752,7 +752,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -894,7 +894,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -904,14 +904,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -922,39 +924,39 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -963,18 +965,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1163,6 +1165,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BCE2EF6-CDA4-4AD0-A42E-3237585D256E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADEC72C-EABA-4F21-8AB5-D28D9F66DD55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1175,14 +1185,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="418c3449-820c-4050-a2e7-95db9dcc5f30"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BCE2EF6-CDA4-4AD0-A42E-3237585D256E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>